<commit_message>
Revertendo layout para versão estável
</commit_message>
<xml_diff>
--- a/produtos_bipados.xlsx
+++ b/produtos_bipados.xlsx
@@ -518,9 +518,13 @@
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>22/05/2025 14:12</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">

</xml_diff>